<commit_message>
Neue Reports und Dateien
</commit_message>
<xml_diff>
--- a/04_Training/train_test_split.xlsx
+++ b/04_Training/train_test_split.xlsx
@@ -1622,7 +1622,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
     </row>

</xml_diff>